<commit_message>
testing, student hour report, and other minor updates
</commit_message>
<xml_diff>
--- a/p3/students.xlsx
+++ b/p3/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/e15/p3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD3C4488-D303-CD4C-A8B1-853CCB1B2D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D889C4B3-77A9-C249-B59D-6DD29704E19D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{6F7FE43B-00CB-FD46-835C-B2A37DA5B158}"/>
   </bookViews>
@@ -433,8 +433,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>